<commit_message>
added licensing columns to mavedb metadata
</commit_message>
<xml_diff>
--- a/data_exploration/MaveDB/mavedb_studies.xlsx
+++ b/data_exploration/MaveDB/mavedb_studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zakirov/Documents/GitHub/PerturbationCatalogue/data_exploration/MaveDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FE5419-CB90-1D4E-BA14-3574EA84199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74E2628-CB8A-444A-92DB-899A9E87208A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12761" uniqueCount="4405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12783" uniqueCount="4409">
   <si>
     <t>dataset_id</t>
   </si>
@@ -13243,6 +13243,18 @@
   </si>
   <si>
     <t>MONDO:0007263</t>
+  </si>
+  <si>
+    <t>license_label</t>
+  </si>
+  <si>
+    <t>license_id</t>
+  </si>
+  <si>
+    <t>SWO:1000049</t>
+  </si>
+  <si>
+    <t>CC0 1.0</t>
   </si>
 </sst>
 </file>
@@ -13310,6 +13322,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -13338,20 +13364,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -13366,8 +13378,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C3C80F3-F87A-E546-ADA5-E9FDB9D045A3}" name="Table1" displayName="Table1" ref="A1:CI1195" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:CI1195" xr:uid="{9C3C80F3-F87A-E546-ADA5-E9FDB9D045A3}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C3C80F3-F87A-E546-ADA5-E9FDB9D045A3}" name="Table1" displayName="Table1" ref="A1:CK1195" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:CK1195" xr:uid="{9C3C80F3-F87A-E546-ADA5-E9FDB9D045A3}">
     <filterColumn colId="0">
       <filters>
         <filter val="urn:mavedb:00000001-a-1"/>
@@ -13383,7 +13395,7 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="87">
+  <tableColumns count="89">
     <tableColumn id="1" xr3:uid="{D4F9CA91-F3A4-084A-B327-E6DA74652796}" name="dataset_id"/>
     <tableColumn id="87" xr3:uid="{1E4F3B44-11CA-0946-BD15-C6B42D5B4808}" name="is_curated"/>
     <tableColumn id="2" xr3:uid="{B1E7FA62-7254-E04F-9F95-8DFE490CD8C9}" name="data_modality"/>
@@ -13471,6 +13483,8 @@
     <tableColumn id="83" xr3:uid="{180E2A03-2E13-D04F-B38C-23B47B2FF1E4}" name="reference_genome_id"/>
     <tableColumn id="84" xr3:uid="{61BFBA9A-E738-CE49-A959-3F4F1D2E5B3F}" name="reference_genome_label"/>
     <tableColumn id="85" xr3:uid="{5F0ED1E5-225D-214D-9D5A-A3969371B167}" name="associated_datasets"/>
+    <tableColumn id="88" xr3:uid="{86D7BAE5-423D-8F4A-927C-2B05B8E55B02}" name="license_label"/>
+    <tableColumn id="89" xr3:uid="{F9DC7C07-C530-294D-B17B-85F669CCCC6D}" name="license_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13763,10 +13777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI1195"/>
+  <dimension ref="A1:CK1195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA1200" sqref="AA1200"/>
+    <sheetView tabSelected="1" topLeftCell="CI1" workbookViewId="0">
+      <selection activeCell="CJ1198" sqref="CJ1198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13857,9 +13871,11 @@
     <col min="85" max="85" width="20.6640625" customWidth="1"/>
     <col min="86" max="86" width="23" customWidth="1"/>
     <col min="87" max="87" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14121,8 +14137,14 @@
       <c r="CI1" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ1" s="1" t="s">
+        <v>4405</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -14252,8 +14274,14 @@
       <c r="CI2" t="s">
         <v>4386</v>
       </c>
-    </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ2" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -14383,8 +14411,14 @@
       <c r="CI3" t="s">
         <v>4374</v>
       </c>
-    </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ3" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -14514,8 +14548,14 @@
       <c r="CI4" t="s">
         <v>4383</v>
       </c>
-    </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ4" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -14642,8 +14682,14 @@
       <c r="CI5" t="s">
         <v>4387</v>
       </c>
-    </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ5" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -14773,8 +14819,14 @@
       <c r="CI6" t="s">
         <v>4390</v>
       </c>
-    </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ6" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -14904,8 +14956,14 @@
       <c r="CI7" t="s">
         <v>4391</v>
       </c>
-    </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ7" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK7" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="8" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -15035,8 +15093,14 @@
       <c r="CI8" t="s">
         <v>4392</v>
       </c>
-    </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ8" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK8" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -15166,8 +15230,14 @@
       <c r="CI9" t="s">
         <v>4393</v>
       </c>
-    </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ9" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK9" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -15291,8 +15361,14 @@
       <c r="CI10" t="s">
         <v>4394</v>
       </c>
-    </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.2">
+      <c r="CJ10" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK10" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -15416,8 +15492,14 @@
       <c r="CI11" t="s">
         <v>4395</v>
       </c>
-    </row>
-    <row r="12" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
+      <c r="CJ11" t="s">
+        <v>4408</v>
+      </c>
+      <c r="CK11" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:89" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -15461,7 +15543,7 @@
         <v>48183</v>
       </c>
     </row>
-    <row r="13" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:89" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -15505,7 +15587,7 @@
         <v>30487</v>
       </c>
     </row>
-    <row r="14" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:89" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -15549,7 +15631,7 @@
         <v>20724</v>
       </c>
     </row>
-    <row r="15" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:89" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -15593,7 +15675,7 @@
         <v>12316</v>
       </c>
     </row>
-    <row r="16" spans="1:87" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:89" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>99</v>
       </c>

</xml_diff>